<commit_message>
add practice and tables
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zby15\Documents\GitHub\program-evaluation-glossary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFEB795-89FD-47C8-99F7-4CA4143BB504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8880A509-AE71-42E8-B72C-D95BD89C7775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Part1</t>
   </si>
@@ -37,16 +37,28 @@
   </si>
   <si>
     <t>Program evaluation standards</t>
+  </si>
+  <si>
+    <t>The Keys to Success</t>
+  </si>
+  <si>
+    <t>Part3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +84,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -354,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,7 +428,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>